<commit_message>
V1 création excel infos générales
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -557,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,13 +565,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -595,9 +595,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -606,9 +603,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB9D900-508B-423C-BE09-F530CF2964C6}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -964,7 +958,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -997,7 +991,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1071,12 +1065,9 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1119,7 +1110,7 @@
       <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1162,7 +1153,7 @@
         <v>41</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I18" s="12"/>
@@ -1175,11 +1166,6 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
@@ -1187,19 +1173,14 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
+      <c r="A23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
@@ -1211,7 +1192,7 @@
       <c r="D24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -1248,7 +1229,7 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="12"/>

</xml_diff>

<commit_message>
refactor(main): séparation en fichiers et fonctions
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="240" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FE0122-6CB0-4C60-B168-7FB98CE23C1D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB9D900-508B-423C-BE09-F530CF2964C6}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Séparation du main et process znieff et commence la gestion des n2000
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griveenvironnement-my.sharepoint.com/personal/marylou_bertin_grive-environnement_fr/Documents/Bureau/Automatisation biblio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FE0122-6CB0-4C60-B168-7FB98CE23C1D}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C242E74-6AAF-4063-86D7-496382D5E901}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="ZNIEFF" sheetId="1" r:id="rId1"/>
+    <sheet name="N2000" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>CORINE biotopes</t>
   </si>
@@ -465,6 +466,42 @@
   </si>
   <si>
     <t xml:space="preserve"> =&gt; Peut y avoir plusieurs lignes réglementation pour une seule espèce. Fusionner les cellules précédentes pour que toutes les réglementations d'une espèce apparaissent sur une seule ligne espèce.</t>
+  </si>
+  <si>
+    <t>Nom zone</t>
+  </si>
+  <si>
+    <t>Type de zone</t>
+  </si>
+  <si>
+    <t>Région biogéographique</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;TYPE&gt;</t>
+  </si>
+  <si>
+    <t>Surface totale</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;SITECODE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;SITE_NAME&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;AREA&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;BIOGEO&gt; &lt;BIOGEOROW&gt; &lt;NAME_FR&gt;</t>
+  </si>
+  <si>
+    <t>Pourcentage</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &gt; &lt;BIOGEO&gt; &lt;BIOGEOROW&gt; &lt;COVER&gt;</t>
   </si>
 </sst>
 </file>
@@ -557,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -603,6 +640,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB9D900-508B-423C-BE09-F530CF2964C6}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,4 +1283,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDA4C-C615-42AB-84E0-A8CD5FE919EF}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour excel modèle
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griveenvironnement-my.sharepoint.com/personal/marylou_bertin_grive-environnement_fr/Documents/Bureau/Automatisation biblio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C242E74-6AAF-4063-86D7-496382D5E901}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C7C590-7C31-48A2-B39C-A05EFCE2A5ED}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
   <si>
     <t>CORINE biotopes</t>
   </si>
@@ -502,6 +502,111 @@
   </si>
   <si>
     <t>&lt;BIOTOPE&gt; &gt; &lt;BIOGEO&gt; &lt;BIOGEOROW&gt; &lt;COVER&gt;</t>
+  </si>
+  <si>
+    <t>Types d’habitats présents sur le site et évaluations</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>Grottes (nombre)</t>
+  </si>
+  <si>
+    <t>Qualité des données</t>
+  </si>
+  <si>
+    <t>Représentativité</t>
+  </si>
+  <si>
+    <t>Superficie relative</t>
+  </si>
+  <si>
+    <t>Conservation</t>
+  </si>
+  <si>
+    <t>Évaluation globale</t>
+  </si>
+  <si>
+    <t>Types d’habitats inscrits à l’annexe I</t>
+  </si>
+  <si>
+    <t>Évaluation du site</t>
+  </si>
+  <si>
+    <t>A|B|C|D</t>
+  </si>
+  <si>
+    <t>A|B|C</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;CD_UE&gt; + &lt;LB_HABDH_FR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;PF&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;AREA&gt;</t>
+  </si>
+  <si>
+    <t>Superficie (% de couverture)</t>
+  </si>
+  <si>
+    <t>Superficie (ha)</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;COVER&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;CAVE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;QUALITY&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;REPRESENT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;REL_SURF&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;CONSERVE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;GLOBAL&gt;</t>
+  </si>
+  <si>
+    <t>Espèces inscrites à l’annexe II de la directive 92/43/CEE et évaluation</t>
+  </si>
+  <si>
+    <t>Nom scientifique</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Unité</t>
+  </si>
+  <si>
+    <t>C|R|V|P</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Isolement</t>
   </si>
 </sst>
 </file>
@@ -594,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -644,11 +749,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,34 +1398,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDA4C-C615-42AB-84E0-A8CD5FE919EF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.08984375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.90625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
         <v>63</v>
       </c>
@@ -1327,13 +1438,12 @@
       <c r="E2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -1341,12 +1451,11 @@
       <c r="F3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>65</v>
       </c>
@@ -1366,8 +1475,164 @@
         <v>73</v>
       </c>
     </row>
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>

</xml_diff>

<commit_message>
Séparation des utils Znieff et commun, et renommage fichiers qui concernent les Znieff
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griveenvironnement-my.sharepoint.com/personal/marylou_bertin_grive-environnement_fr/Documents/Bureau/Automatisation biblio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C7C590-7C31-48A2-B39C-A05EFCE2A5ED}"/>
+  <xr:revisionPtr revIDLastSave="651" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A22615E-06A4-4F96-A0BF-599BFE7024FD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
   <si>
     <t>CORINE biotopes</t>
   </si>
@@ -600,13 +600,139 @@
     <t>Unité</t>
   </si>
   <si>
-    <t>C|R|V|P</t>
-  </si>
-  <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>Isolement</t>
+  </si>
+  <si>
+    <t>Catégorie (C|R|V|P)</t>
+  </si>
+  <si>
+    <t>Population (A|B|C|D)</t>
+  </si>
+  <si>
+    <t>Espèce</t>
+  </si>
+  <si>
+    <t>Population présente sur le site</t>
+  </si>
+  <si>
+    <t>Taille</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;TAXGROUP&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;CODE_N2000&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;NOM&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;TYPE&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;SIZE_MIN&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;SIZE_MAX&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;CAT_POP&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;UNIT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;QUALITY&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;POPULATION&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;CONSERVE&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;ISOLATION&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;GLOBAL&gt;</t>
+  </si>
+  <si>
+    <t>Autres espèces importantes de faune et de flore</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Annexe Directive Habitat</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Autres catégories</t>
+  </si>
+  <si>
+    <t>Motivation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;TAXGROUP&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;LB_NOM&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;SIZE_MIN&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;SIZE_MAX&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;UNIT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;CAT_POP&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;ANNEX_IV&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;ANNEX_V&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;A&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;B&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;C&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;SPECIES_OTHER&gt; &lt;SPECIES_OTHER_ROW&gt; &lt;D&gt;</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Int</t>
   </si>
 </sst>
 </file>
@@ -699,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,8 +872,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -755,11 +884,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,56 +1530,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDA4C-C615-42AB-84E0-A8CD5FE919EF}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="37" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="64.08984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="65" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="42.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.90625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="4" t="s">
         <v>72</v>
       </c>
@@ -1476,61 +1610,61 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="18" t="s">
         <v>79</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1545,6 +1679,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>88</v>
       </c>
@@ -1576,54 +1713,414 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B21" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="21"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B22" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="G22" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>83</v>
+      <c r="H22" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="37">
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="B7:G7"/>
@@ -1633,11 +2130,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout en tete tableau N2000
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="651" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A22615E-06A4-4F96-A0BF-599BFE7024FD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
   <sheets>
     <sheet name="ZNIEFF" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,20 +878,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1532,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDA4C-C615-42AB-84E0-A8CD5FE919EF}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="37" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,56 +1612,56 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="19" t="s">
         <v>79</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1679,7 +1676,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1714,7 +1711,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1755,78 +1752,78 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="1" t="s">
         <v>103</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="1" t="s">
         <v>82</v>
       </c>
@@ -1838,7 +1835,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1882,7 +1879,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1931,65 +1928,64 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18" t="s">
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18" t="s">
+      <c r="I22" s="19"/>
+      <c r="J22" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1" t="s">
         <v>126</v>
       </c>
@@ -2010,7 +2006,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2051,7 +2047,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2093,16 +2089,20 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:B16"/>
@@ -2116,20 +2116,16 @@
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout de commentaires et finission des tableaux N2000
</commit_message>
<xml_diff>
--- a/Modèle excel.xlsx
+++ b/Modèle excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griveenvironnement-my.sharepoint.com/personal/marylou_bertin_grive-environnement_fr/Documents/Bureau/Automatisation biblio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarylouBERTIN\Documents\Automatisation-biblio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="651" documentId="8_{8BA710CA-7BFF-422D-97E9-A3445B6F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A22615E-06A4-4F96-A0BF-599BFE7024FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B0E0CE-E297-4BA2-90FA-AE89293D732B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{64A6EA69-29D9-4568-A2D1-7E13428A705C}"/>
   </bookViews>
   <sheets>
     <sheet name="ZNIEFF" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t>CORINE biotopes</t>
   </si>
@@ -504,9 +504,6 @@
     <t>&lt;BIOTOPE&gt; &gt; &lt;BIOGEO&gt; &lt;BIOGEOROW&gt; &lt;COVER&gt;</t>
   </si>
   <si>
-    <t>Types d’habitats présents sur le site et évaluations</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -582,9 +579,6 @@
     <t>&lt;BIOTOPE&gt; &lt;HABIT1&gt;  &lt;HABIT1_ROW&gt; &lt;GLOBAL&gt;</t>
   </si>
   <si>
-    <t>Espèces inscrites à l’annexe II de la directive 92/43/CEE et évaluation</t>
-  </si>
-  <si>
     <t>Nom scientifique</t>
   </si>
   <si>
@@ -655,9 +649,6 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;SPECIES&gt; &lt;SPECIES_ROW&gt; &lt;GLOBAL&gt;</t>
-  </si>
-  <si>
-    <t>Autres espèces importantes de faune et de flore</t>
   </si>
   <si>
     <t>IV</t>
@@ -825,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,23 +863,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,141 +1509,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDA4C-C615-42AB-84E0-A8CD5FE919EF}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="42.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="58" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="42.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.90625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="19" t="s">
+      <c r="H8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="19"/>
       <c r="H9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1671,13 +1645,10 @@
       <c r="J9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
-        <v>30</v>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>88</v>
@@ -1686,7 +1657,7 @@
         <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>93</v>
@@ -1706,426 +1677,395 @@
       <c r="J10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="D15" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="19" t="s">
+      <c r="B17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>117</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>118</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>102</v>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>147</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19" t="s">
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
-        <v>102</v>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>